<commit_message>
Scrum Update & Invulblad leeggemaakt voor volgende scrums
</commit_message>
<xml_diff>
--- a/Algemeen/Scrumlog/Invulblad.xlsx
+++ b/Algemeen/Scrumlog/Invulblad.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\FPS\Algemeen\Scrumlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\super\Desktop\GitHub\Team-Asylum3\Algemeen\Scrumlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Week #</t>
   </si>
@@ -81,57 +81,12 @@
   </si>
   <si>
     <t>Rief , Michiel , Robin</t>
-  </si>
-  <si>
-    <t>Shotgun</t>
-  </si>
-  <si>
-    <t>Gunscript</t>
-  </si>
-  <si>
-    <t>Player Controller</t>
-  </si>
-  <si>
-    <t>unwrap pistol</t>
-  </si>
-  <si>
-    <t>main menu</t>
-  </si>
-  <si>
-    <t>Main Character</t>
-  </si>
-  <si>
-    <t>Muren en Textures</t>
-  </si>
-  <si>
-    <t>Shotgun texture</t>
-  </si>
-  <si>
-    <t>Planning volgen</t>
-  </si>
-  <si>
-    <t>Planning Maken</t>
-  </si>
-  <si>
-    <t>Texture en Animatie</t>
-  </si>
-  <si>
-    <t>Main Character]</t>
-  </si>
-  <si>
-    <t>Waarom zo boos?(-zine)</t>
-  </si>
-  <si>
-    <t>Anxiety</t>
-  </si>
-  <si>
-    <t>Team Spirit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,12 +554,12 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -618,7 +573,7 @@
       <c r="G1" s="8"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
@@ -632,7 +587,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -646,7 +601,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -660,7 +615,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="12" t="s">
@@ -672,105 +627,91 @@
       <c r="G5" s="9"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="12" t="s">
@@ -782,105 +723,91 @@
       <c r="G13" s="9"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="7"/>
-      <c r="C18" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="12" t="s">
@@ -892,7 +819,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -904,35 +831,31 @@
       <c r="G22" s="8"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -944,7 +867,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>8</v>
       </c>
@@ -956,7 +879,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
@@ -968,7 +891,7 @@
       <c r="G27" s="9"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
@@ -980,21 +903,19 @@
       <c r="G28" s="9"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="C29" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="9"/>
@@ -1004,7 +925,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -1016,7 +937,7 @@
       <c r="G31" s="8"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="9"/>

</xml_diff>